<commit_message>
COM and Motor Driver Updates
Added Initialization command from Pi to MSP (see
"communication_protocol.xlsx".  Also added easy switching between motor
stepping modes.
</commit_message>
<xml_diff>
--- a/Laser_Engraver_Embedded/communication_protocol.xlsx
+++ b/Laser_Engraver_Embedded/communication_protocol.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Laser Engraver Commands" sheetId="4" r:id="rId2"/>
     <sheet name="Communication Character Defs" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="100">
   <si>
     <t>Bit7</t>
   </si>
@@ -206,9 +206,6 @@
     <t>MSP has encountered a problem and needs to stop the burn (payload indicates failure condition)</t>
   </si>
   <si>
-    <t>MSP is initialized and ready to burn an image</t>
-  </si>
-  <si>
     <t>Pi will commence sending burn pixel commands</t>
   </si>
   <si>
@@ -309,6 +306,21 @@
   </si>
   <si>
     <t>End Picture</t>
+  </si>
+  <si>
+    <t>ACK RX PACKET  (MSP to Pi)</t>
+  </si>
+  <si>
+    <t>NAK RX PACKET  (MSP to Pi)</t>
+  </si>
+  <si>
+    <t>INIT</t>
+  </si>
+  <si>
+    <t>Pi or MSP is initialized and ready to proceed</t>
+  </si>
+  <si>
+    <t>Pi has correctly initialized and is ready to start communicating with the MSP</t>
   </si>
 </sst>
 </file>
@@ -587,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -704,6 +716,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -725,6 +740,18 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -735,18 +762,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1058,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,6 +1101,7 @@
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="24"/>
       <c r="K1" s="24"/>
       <c r="L1" s="24"/>
@@ -1094,24 +1110,25 @@
       <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="A2" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
       <c r="H2" s="24"/>
-      <c r="J2" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
@@ -1122,6 +1139,7 @@
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="24"/>
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
@@ -1133,24 +1151,25 @@
       <c r="A4" s="24"/>
       <c r="B4" s="22"/>
       <c r="C4" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>74</v>
-      </c>
       <c r="E4" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="24"/>
       <c r="K4" s="22"/>
       <c r="L4" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M4" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N4" s="23"/>
       <c r="O4" s="24"/>
@@ -1164,6 +1183,7 @@
       <c r="F5" s="28"/>
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
       <c r="J5" s="24"/>
       <c r="K5" s="26"/>
       <c r="L5" s="27"/>
@@ -1174,20 +1194,21 @@
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="29"/>
-      <c r="C6" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
+      <c r="C6" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="30"/>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="K6" s="29"/>
-      <c r="L6" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="M6" s="41"/>
+      <c r="L6" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="M6" s="42"/>
       <c r="N6" s="30"/>
       <c r="O6" s="24"/>
     </row>
@@ -1200,6 +1221,7 @@
       <c r="F7" s="28"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
       <c r="J7" s="24"/>
       <c r="K7" s="26"/>
       <c r="L7" s="27"/>
@@ -1209,114 +1231,119 @@
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="5" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="24"/>
-      <c r="K8" s="3"/>
+      <c r="K8" s="26"/>
       <c r="L8" s="5" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="N8" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="N8" s="28"/>
       <c r="O8" s="24"/>
     </row>
-    <row r="9" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
+      <c r="C9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>32</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="25"/>
+      <c r="L9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>90</v>
+      </c>
       <c r="N9" s="6"/>
       <c r="O9" s="24"/>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
       <c r="F10" s="6"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="24"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="M10" s="42"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="25"/>
       <c r="N10" s="6"/>
       <c r="O10" s="24"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>34</v>
-      </c>
+      <c r="C11" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="6"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="24"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="M11" s="37" t="s">
-        <v>90</v>
-      </c>
+      <c r="L11" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="M11" s="43"/>
       <c r="N11" s="6"/>
       <c r="O11" s="24"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>25</v>
+      <c r="C12" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="24"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="M12" s="38" t="s">
-        <v>92</v>
+      <c r="L12" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="M12" s="37" t="s">
+        <v>89</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="24"/>
@@ -1325,24 +1352,25 @@
       <c r="A13" s="24"/>
       <c r="B13" s="3"/>
       <c r="C13" s="13" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="24"/>
       <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
       <c r="J13" s="24"/>
       <c r="K13" s="3"/>
       <c r="L13" s="13" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="M13" s="38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="24"/>
@@ -1351,21 +1379,22 @@
       <c r="A14" s="24"/>
       <c r="B14" s="3"/>
       <c r="C14" s="13" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>80</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="24"/>
       <c r="K14" s="3"/>
       <c r="L14" s="13" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="M14" s="38" t="s">
         <v>92</v>
@@ -1377,24 +1406,25 @@
       <c r="A15" s="24"/>
       <c r="B15" s="3"/>
       <c r="C15" s="13" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="3"/>
       <c r="L15" s="13" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="M15" s="38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="24"/>
@@ -1403,24 +1433,25 @@
       <c r="A16" s="24"/>
       <c r="B16" s="3"/>
       <c r="C16" s="13" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="E16" s="38" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="24"/>
       <c r="K16" s="3"/>
       <c r="L16" s="13" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="M16" s="38" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="24"/>
@@ -1429,24 +1460,25 @@
       <c r="A17" s="24"/>
       <c r="B17" s="3"/>
       <c r="C17" s="13" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="24"/>
       <c r="K17" s="3"/>
       <c r="L17" s="13" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="M17" s="38" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="24"/>
@@ -1454,239 +1486,279 @@
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>36</v>
+      <c r="C18" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>77</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
       <c r="J18" s="24"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="M18" s="39" t="s">
-        <v>95</v>
+      <c r="L18" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="M18" s="38" t="s">
+        <v>93</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="24"/>
     </row>
-    <row r="19" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
+      <c r="C19" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>36</v>
+      </c>
       <c r="F19" s="6"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="24"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="25"/>
+      <c r="L19" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="M19" s="39" t="s">
+        <v>94</v>
+      </c>
       <c r="N19" s="6"/>
       <c r="O19" s="24"/>
     </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
       <c r="F20" s="6"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
       <c r="J20" s="24"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="M20" s="42"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="25"/>
       <c r="N20" s="6"/>
       <c r="O20" s="24"/>
     </row>
-    <row r="21" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
+      <c r="C21" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="6"/>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="24"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="25"/>
+      <c r="L21" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="M21" s="43"/>
       <c r="N21" s="6"/>
       <c r="O21" s="24"/>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
       <c r="F22" s="6"/>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="24"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="M22" s="42"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="25"/>
       <c r="N22" s="6"/>
       <c r="O22" s="24"/>
     </row>
-    <row r="23" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
+      <c r="C23" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="6"/>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="24"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="25"/>
+      <c r="L23" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="M23" s="43"/>
       <c r="N23" s="6"/>
       <c r="O23" s="24"/>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
       <c r="F24" s="6"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="24"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24" s="43"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="25"/>
       <c r="N24" s="6"/>
       <c r="O24" s="24"/>
     </row>
-    <row r="25" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="C25" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
       <c r="F25" s="6"/>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="24"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="25"/>
+      <c r="L25" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M25" s="44"/>
       <c r="N25" s="6"/>
       <c r="O25" s="24"/>
     </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="30"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="24"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="M26" s="41"/>
-      <c r="N26" s="30"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="6"/>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="10"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="30"/>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
       <c r="J27" s="24"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="10"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="M27" s="42"/>
+      <c r="N27" s="30"/>
       <c r="O27" s="24"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="10"/>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
       <c r="J28" s="24"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="10"/>
       <c r="O28" s="24"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
       <c r="G29" s="24"/>
       <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
       <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
       <c r="O29" s="24"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L23:M23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1694,8 +1766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L244"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R135" sqref="R135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1723,17 +1795,17 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -1749,32 +1821,32 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="50"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="47"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
@@ -1815,18 +1887,18 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
@@ -1867,18 +1939,18 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="47"/>
     </row>
     <row r="14" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15"/>
@@ -1905,15 +1977,15 @@
       <c r="E15" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="50"/>
-      <c r="H15" s="48" t="s">
+      <c r="G15" s="55"/>
+      <c r="H15" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="55"/>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
@@ -1960,16 +2032,16 @@
       <c r="B18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="50"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="55"/>
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -2016,18 +2088,18 @@
       <c r="B21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="48" t="s">
+      <c r="D21" s="55"/>
+      <c r="E21" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="50"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="55"/>
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -2074,15 +2146,15 @@
       <c r="B24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="50"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="55"/>
       <c r="J24" s="12" t="s">
         <v>49</v>
       </c>
@@ -2129,18 +2201,18 @@
       <c r="K26" s="10"/>
     </row>
     <row r="27" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="47"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="13"/>
@@ -2181,18 +2253,18 @@
       <c r="K30" s="10"/>
     </row>
     <row r="31" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="47"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
@@ -2214,12 +2286,12 @@
       <c r="D33" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="47" t="s">
+      <c r="E33" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
       <c r="I33" s="14" t="s">
         <v>38</v>
       </c>
@@ -2297,18 +2369,18 @@
       <c r="K36" s="10"/>
     </row>
     <row r="37" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="47"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="13"/>
@@ -2395,18 +2467,18 @@
       <c r="K42" s="6"/>
     </row>
     <row r="43" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="47"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="13"/>
@@ -2505,32 +2577,32 @@
       <c r="K49" s="1"/>
     </row>
     <row r="50" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="51" t="s">
+      <c r="B50" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C50" s="52"/>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="52"/>
-      <c r="I50" s="52"/>
-      <c r="J50" s="52"/>
-      <c r="K50" s="53"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="50"/>
     </row>
     <row r="51" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="44" t="s">
+      <c r="B51" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="45"/>
-      <c r="J51" s="45"/>
-      <c r="K51" s="46"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="47"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
@@ -2571,18 +2643,18 @@
       <c r="K54" s="10"/>
     </row>
     <row r="55" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="44" t="s">
+      <c r="B55" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="45"/>
-      <c r="J55" s="45"/>
-      <c r="K55" s="46"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="46"/>
+      <c r="I55" s="46"/>
+      <c r="J55" s="46"/>
+      <c r="K55" s="47"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
@@ -2623,18 +2695,18 @@
       <c r="K58" s="10"/>
     </row>
     <row r="59" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B59" s="44" t="s">
+      <c r="B59" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="45"/>
-      <c r="J59" s="45"/>
-      <c r="K59" s="46"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="47"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="15"/>
@@ -2675,18 +2747,18 @@
       <c r="K62" s="10"/>
     </row>
     <row r="63" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B63" s="44" t="s">
+      <c r="B63" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="45"/>
-      <c r="F63" s="45"/>
-      <c r="G63" s="45"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="45"/>
-      <c r="J63" s="45"/>
-      <c r="K63" s="46"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
+      <c r="J63" s="46"/>
+      <c r="K63" s="47"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="13"/>
@@ -2727,18 +2799,18 @@
       <c r="K66" s="10"/>
     </row>
     <row r="67" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B67" s="44" t="s">
+      <c r="B67" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="C67" s="45"/>
-      <c r="D67" s="45"/>
-      <c r="E67" s="45"/>
-      <c r="F67" s="45"/>
-      <c r="G67" s="45"/>
-      <c r="H67" s="45"/>
-      <c r="I67" s="45"/>
-      <c r="J67" s="45"/>
-      <c r="K67" s="46"/>
+      <c r="C67" s="46"/>
+      <c r="D67" s="46"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="46"/>
+      <c r="I67" s="46"/>
+      <c r="J67" s="46"/>
+      <c r="K67" s="47"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="13"/>
@@ -2819,18 +2891,18 @@
       <c r="K72" s="10"/>
     </row>
     <row r="73" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B73" s="44" t="s">
+      <c r="B73" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C73" s="45"/>
-      <c r="D73" s="45"/>
-      <c r="E73" s="45"/>
-      <c r="F73" s="45"/>
-      <c r="G73" s="45"/>
-      <c r="H73" s="45"/>
-      <c r="I73" s="45"/>
-      <c r="J73" s="45"/>
-      <c r="K73" s="46"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="46"/>
+      <c r="E73" s="46"/>
+      <c r="F73" s="46"/>
+      <c r="G73" s="46"/>
+      <c r="H73" s="46"/>
+      <c r="I73" s="46"/>
+      <c r="J73" s="46"/>
+      <c r="K73" s="47"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" s="13"/>
@@ -2917,18 +2989,18 @@
       <c r="K78" s="6"/>
     </row>
     <row r="79" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B79" s="44" t="s">
+      <c r="B79" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C79" s="45"/>
-      <c r="D79" s="45"/>
-      <c r="E79" s="45"/>
-      <c r="F79" s="45"/>
-      <c r="G79" s="45"/>
-      <c r="H79" s="45"/>
-      <c r="I79" s="45"/>
-      <c r="J79" s="45"/>
-      <c r="K79" s="46"/>
+      <c r="C79" s="46"/>
+      <c r="D79" s="46"/>
+      <c r="E79" s="46"/>
+      <c r="F79" s="46"/>
+      <c r="G79" s="46"/>
+      <c r="H79" s="46"/>
+      <c r="I79" s="46"/>
+      <c r="J79" s="46"/>
+      <c r="K79" s="47"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" s="13"/>
@@ -3027,32 +3099,32 @@
       <c r="K85" s="5"/>
     </row>
     <row r="86" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B86" s="51" t="s">
+      <c r="B86" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C86" s="52"/>
-      <c r="D86" s="52"/>
-      <c r="E86" s="52"/>
-      <c r="F86" s="52"/>
-      <c r="G86" s="52"/>
-      <c r="H86" s="52"/>
-      <c r="I86" s="52"/>
-      <c r="J86" s="52"/>
-      <c r="K86" s="53"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="49"/>
+      <c r="E86" s="49"/>
+      <c r="F86" s="49"/>
+      <c r="G86" s="49"/>
+      <c r="H86" s="49"/>
+      <c r="I86" s="49"/>
+      <c r="J86" s="49"/>
+      <c r="K86" s="50"/>
     </row>
     <row r="87" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B87" s="44" t="s">
+      <c r="B87" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C87" s="45"/>
-      <c r="D87" s="45"/>
-      <c r="E87" s="45"/>
-      <c r="F87" s="45"/>
-      <c r="G87" s="45"/>
-      <c r="H87" s="45"/>
-      <c r="I87" s="45"/>
-      <c r="J87" s="45"/>
-      <c r="K87" s="46"/>
+      <c r="C87" s="46"/>
+      <c r="D87" s="46"/>
+      <c r="E87" s="46"/>
+      <c r="F87" s="46"/>
+      <c r="G87" s="46"/>
+      <c r="H87" s="46"/>
+      <c r="I87" s="46"/>
+      <c r="J87" s="46"/>
+      <c r="K87" s="47"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" s="3"/>
@@ -3093,18 +3165,18 @@
       <c r="K90" s="10"/>
     </row>
     <row r="91" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B91" s="44" t="s">
+      <c r="B91" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C91" s="45"/>
-      <c r="D91" s="45"/>
-      <c r="E91" s="45"/>
-      <c r="F91" s="45"/>
-      <c r="G91" s="45"/>
-      <c r="H91" s="45"/>
-      <c r="I91" s="45"/>
-      <c r="J91" s="45"/>
-      <c r="K91" s="46"/>
+      <c r="C91" s="46"/>
+      <c r="D91" s="46"/>
+      <c r="E91" s="46"/>
+      <c r="F91" s="46"/>
+      <c r="G91" s="46"/>
+      <c r="H91" s="46"/>
+      <c r="I91" s="46"/>
+      <c r="J91" s="46"/>
+      <c r="K91" s="47"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B92" s="3"/>
@@ -3145,18 +3217,18 @@
       <c r="K94" s="10"/>
     </row>
     <row r="95" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B95" s="44" t="s">
+      <c r="B95" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C95" s="45"/>
-      <c r="D95" s="45"/>
-      <c r="E95" s="45"/>
-      <c r="F95" s="45"/>
-      <c r="G95" s="45"/>
-      <c r="H95" s="45"/>
-      <c r="I95" s="45"/>
-      <c r="J95" s="45"/>
-      <c r="K95" s="46"/>
+      <c r="C95" s="46"/>
+      <c r="D95" s="46"/>
+      <c r="E95" s="46"/>
+      <c r="F95" s="46"/>
+      <c r="G95" s="46"/>
+      <c r="H95" s="46"/>
+      <c r="I95" s="46"/>
+      <c r="J95" s="46"/>
+      <c r="K95" s="47"/>
     </row>
     <row r="96" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="15"/>
@@ -3174,16 +3246,16 @@
       <c r="B97" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C97" s="48" t="s">
+      <c r="C97" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="D97" s="49"/>
-      <c r="E97" s="49"/>
-      <c r="F97" s="49"/>
-      <c r="G97" s="49"/>
-      <c r="H97" s="49"/>
-      <c r="I97" s="49"/>
-      <c r="J97" s="50"/>
+      <c r="D97" s="54"/>
+      <c r="E97" s="54"/>
+      <c r="F97" s="54"/>
+      <c r="G97" s="54"/>
+      <c r="H97" s="54"/>
+      <c r="I97" s="54"/>
+      <c r="J97" s="55"/>
       <c r="K97" s="6"/>
     </row>
     <row r="98" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3227,18 +3299,18 @@
       <c r="K99" s="10"/>
     </row>
     <row r="100" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B100" s="44" t="s">
+      <c r="B100" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C100" s="45"/>
-      <c r="D100" s="45"/>
-      <c r="E100" s="45"/>
-      <c r="F100" s="45"/>
-      <c r="G100" s="45"/>
-      <c r="H100" s="45"/>
-      <c r="I100" s="45"/>
-      <c r="J100" s="45"/>
-      <c r="K100" s="46"/>
+      <c r="C100" s="46"/>
+      <c r="D100" s="46"/>
+      <c r="E100" s="46"/>
+      <c r="F100" s="46"/>
+      <c r="G100" s="46"/>
+      <c r="H100" s="46"/>
+      <c r="I100" s="46"/>
+      <c r="J100" s="46"/>
+      <c r="K100" s="47"/>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B101" s="13"/>
@@ -3279,18 +3351,18 @@
       <c r="K103" s="10"/>
     </row>
     <row r="104" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B104" s="44" t="s">
+      <c r="B104" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="C104" s="45"/>
-      <c r="D104" s="45"/>
-      <c r="E104" s="45"/>
-      <c r="F104" s="45"/>
-      <c r="G104" s="45"/>
-      <c r="H104" s="45"/>
-      <c r="I104" s="45"/>
-      <c r="J104" s="45"/>
-      <c r="K104" s="46"/>
+      <c r="C104" s="46"/>
+      <c r="D104" s="46"/>
+      <c r="E104" s="46"/>
+      <c r="F104" s="46"/>
+      <c r="G104" s="46"/>
+      <c r="H104" s="46"/>
+      <c r="I104" s="46"/>
+      <c r="J104" s="46"/>
+      <c r="K104" s="47"/>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B105" s="13"/>
@@ -3383,18 +3455,18 @@
       <c r="K109" s="10"/>
     </row>
     <row r="110" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B110" s="44" t="s">
+      <c r="B110" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C110" s="45"/>
-      <c r="D110" s="45"/>
-      <c r="E110" s="45"/>
-      <c r="F110" s="45"/>
-      <c r="G110" s="45"/>
-      <c r="H110" s="45"/>
-      <c r="I110" s="45"/>
-      <c r="J110" s="45"/>
-      <c r="K110" s="46"/>
+      <c r="C110" s="46"/>
+      <c r="D110" s="46"/>
+      <c r="E110" s="46"/>
+      <c r="F110" s="46"/>
+      <c r="G110" s="46"/>
+      <c r="H110" s="46"/>
+      <c r="I110" s="46"/>
+      <c r="J110" s="46"/>
+      <c r="K110" s="47"/>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B111" s="13"/>
@@ -3481,18 +3553,18 @@
       <c r="K115" s="6"/>
     </row>
     <row r="116" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B116" s="44" t="s">
+      <c r="B116" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C116" s="45"/>
-      <c r="D116" s="45"/>
-      <c r="E116" s="45"/>
-      <c r="F116" s="45"/>
-      <c r="G116" s="45"/>
-      <c r="H116" s="45"/>
-      <c r="I116" s="45"/>
-      <c r="J116" s="45"/>
-      <c r="K116" s="46"/>
+      <c r="C116" s="46"/>
+      <c r="D116" s="46"/>
+      <c r="E116" s="46"/>
+      <c r="F116" s="46"/>
+      <c r="G116" s="46"/>
+      <c r="H116" s="46"/>
+      <c r="I116" s="46"/>
+      <c r="J116" s="46"/>
+      <c r="K116" s="47"/>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B117" s="13"/>
@@ -3591,32 +3663,32 @@
       <c r="K122" s="1"/>
     </row>
     <row r="123" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B123" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="C123" s="52"/>
-      <c r="D123" s="52"/>
-      <c r="E123" s="52"/>
-      <c r="F123" s="52"/>
-      <c r="G123" s="52"/>
-      <c r="H123" s="52"/>
-      <c r="I123" s="52"/>
-      <c r="J123" s="52"/>
-      <c r="K123" s="53"/>
+      <c r="B123" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C123" s="49"/>
+      <c r="D123" s="49"/>
+      <c r="E123" s="49"/>
+      <c r="F123" s="49"/>
+      <c r="G123" s="49"/>
+      <c r="H123" s="49"/>
+      <c r="I123" s="49"/>
+      <c r="J123" s="49"/>
+      <c r="K123" s="50"/>
     </row>
     <row r="124" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B124" s="44" t="s">
+      <c r="B124" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C124" s="45"/>
-      <c r="D124" s="45"/>
-      <c r="E124" s="45"/>
-      <c r="F124" s="45"/>
-      <c r="G124" s="45"/>
-      <c r="H124" s="45"/>
-      <c r="I124" s="45"/>
-      <c r="J124" s="45"/>
-      <c r="K124" s="46"/>
+      <c r="C124" s="46"/>
+      <c r="D124" s="46"/>
+      <c r="E124" s="46"/>
+      <c r="F124" s="46"/>
+      <c r="G124" s="46"/>
+      <c r="H124" s="46"/>
+      <c r="I124" s="46"/>
+      <c r="J124" s="46"/>
+      <c r="K124" s="47"/>
     </row>
     <row r="125" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B125" s="3"/>
@@ -3633,7 +3705,7 @@
     <row r="126" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B126" s="3"/>
       <c r="C126" s="4" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
@@ -3657,18 +3729,18 @@
       <c r="K127" s="10"/>
     </row>
     <row r="128" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B128" s="44" t="s">
+      <c r="B128" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C128" s="45"/>
-      <c r="D128" s="45"/>
-      <c r="E128" s="45"/>
-      <c r="F128" s="45"/>
-      <c r="G128" s="45"/>
-      <c r="H128" s="45"/>
-      <c r="I128" s="45"/>
-      <c r="J128" s="45"/>
-      <c r="K128" s="46"/>
+      <c r="C128" s="46"/>
+      <c r="D128" s="46"/>
+      <c r="E128" s="46"/>
+      <c r="F128" s="46"/>
+      <c r="G128" s="46"/>
+      <c r="H128" s="46"/>
+      <c r="I128" s="46"/>
+      <c r="J128" s="46"/>
+      <c r="K128" s="47"/>
     </row>
     <row r="129" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B129" s="3"/>
@@ -3709,29 +3781,29 @@
       <c r="K131" s="10"/>
     </row>
     <row r="132" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B132" s="44" t="s">
+      <c r="B132" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C132" s="45"/>
-      <c r="D132" s="45"/>
-      <c r="E132" s="45"/>
-      <c r="F132" s="45"/>
-      <c r="G132" s="45"/>
-      <c r="H132" s="45"/>
-      <c r="I132" s="45"/>
-      <c r="J132" s="45"/>
-      <c r="K132" s="46"/>
+      <c r="C132" s="46"/>
+      <c r="D132" s="46"/>
+      <c r="E132" s="46"/>
+      <c r="F132" s="46"/>
+      <c r="G132" s="46"/>
+      <c r="H132" s="46"/>
+      <c r="I132" s="46"/>
+      <c r="J132" s="46"/>
+      <c r="K132" s="47"/>
     </row>
     <row r="133" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B133" s="15"/>
-      <c r="C133" s="16"/>
-      <c r="D133" s="16"/>
-      <c r="E133" s="16"/>
-      <c r="F133" s="16"/>
-      <c r="G133" s="16"/>
-      <c r="H133" s="16"/>
-      <c r="I133" s="16"/>
-      <c r="J133" s="16"/>
+      <c r="C133" s="40"/>
+      <c r="D133" s="40"/>
+      <c r="E133" s="40"/>
+      <c r="F133" s="40"/>
+      <c r="G133" s="40"/>
+      <c r="H133" s="40"/>
+      <c r="I133" s="40"/>
+      <c r="J133" s="40"/>
       <c r="K133" s="6"/>
     </row>
     <row r="134" spans="2:11" x14ac:dyDescent="0.25">
@@ -3739,13 +3811,13 @@
       <c r="C134" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D134" s="16"/>
-      <c r="E134" s="16"/>
-      <c r="F134" s="16"/>
-      <c r="G134" s="16"/>
-      <c r="H134" s="16"/>
-      <c r="I134" s="16"/>
-      <c r="J134" s="16"/>
+      <c r="D134" s="40"/>
+      <c r="E134" s="40"/>
+      <c r="F134" s="40"/>
+      <c r="G134" s="40"/>
+      <c r="H134" s="40"/>
+      <c r="I134" s="40"/>
+      <c r="J134" s="40"/>
       <c r="K134" s="6"/>
     </row>
     <row r="135" spans="2:11" x14ac:dyDescent="0.25">
@@ -3761,18 +3833,18 @@
       <c r="K135" s="10"/>
     </row>
     <row r="136" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B136" s="44" t="s">
+      <c r="B136" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C136" s="45"/>
-      <c r="D136" s="45"/>
-      <c r="E136" s="45"/>
-      <c r="F136" s="45"/>
-      <c r="G136" s="45"/>
-      <c r="H136" s="45"/>
-      <c r="I136" s="45"/>
-      <c r="J136" s="45"/>
-      <c r="K136" s="46"/>
+      <c r="C136" s="46"/>
+      <c r="D136" s="46"/>
+      <c r="E136" s="46"/>
+      <c r="F136" s="46"/>
+      <c r="G136" s="46"/>
+      <c r="H136" s="46"/>
+      <c r="I136" s="46"/>
+      <c r="J136" s="46"/>
+      <c r="K136" s="47"/>
     </row>
     <row r="137" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="13"/>
@@ -3791,13 +3863,13 @@
       <c r="C138" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D138" s="16"/>
-      <c r="E138" s="16"/>
-      <c r="F138" s="16"/>
-      <c r="G138" s="16"/>
-      <c r="H138" s="16"/>
-      <c r="I138" s="54"/>
-      <c r="J138" s="54"/>
+      <c r="D138" s="40"/>
+      <c r="E138" s="40"/>
+      <c r="F138" s="40"/>
+      <c r="G138" s="40"/>
+      <c r="H138" s="40"/>
+      <c r="I138" s="51"/>
+      <c r="J138" s="51"/>
       <c r="K138" s="6"/>
     </row>
     <row r="139" spans="2:11" x14ac:dyDescent="0.25">
@@ -3813,18 +3885,18 @@
       <c r="K139" s="10"/>
     </row>
     <row r="140" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B140" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="C140" s="45"/>
-      <c r="D140" s="45"/>
-      <c r="E140" s="45"/>
-      <c r="F140" s="45"/>
-      <c r="G140" s="45"/>
-      <c r="H140" s="45"/>
-      <c r="I140" s="45"/>
-      <c r="J140" s="45"/>
-      <c r="K140" s="46"/>
+      <c r="B140" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C140" s="46"/>
+      <c r="D140" s="46"/>
+      <c r="E140" s="46"/>
+      <c r="F140" s="46"/>
+      <c r="G140" s="46"/>
+      <c r="H140" s="46"/>
+      <c r="I140" s="46"/>
+      <c r="J140" s="46"/>
+      <c r="K140" s="47"/>
     </row>
     <row r="141" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B141" s="13"/>
@@ -3905,18 +3977,18 @@
       <c r="K145" s="6"/>
     </row>
     <row r="146" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B146" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="C146" s="45"/>
-      <c r="D146" s="45"/>
-      <c r="E146" s="45"/>
-      <c r="F146" s="45"/>
-      <c r="G146" s="45"/>
-      <c r="H146" s="45"/>
-      <c r="I146" s="45"/>
-      <c r="J146" s="45"/>
-      <c r="K146" s="46"/>
+      <c r="B146" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C146" s="46"/>
+      <c r="D146" s="46"/>
+      <c r="E146" s="46"/>
+      <c r="F146" s="46"/>
+      <c r="G146" s="46"/>
+      <c r="H146" s="46"/>
+      <c r="I146" s="46"/>
+      <c r="J146" s="46"/>
+      <c r="K146" s="47"/>
     </row>
     <row r="147" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B147" s="13"/>
@@ -3965,8 +4037,8 @@
         <v>16</v>
       </c>
       <c r="G149" s="14"/>
-      <c r="H149" s="16"/>
-      <c r="I149" s="16"/>
+      <c r="H149" s="40"/>
+      <c r="I149" s="40"/>
       <c r="J149" s="1"/>
       <c r="K149" s="6"/>
     </row>
@@ -4003,18 +4075,18 @@
       <c r="K151" s="6"/>
     </row>
     <row r="152" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B152" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="C152" s="45"/>
-      <c r="D152" s="45"/>
-      <c r="E152" s="45"/>
-      <c r="F152" s="45"/>
-      <c r="G152" s="45"/>
-      <c r="H152" s="45"/>
-      <c r="I152" s="45"/>
-      <c r="J152" s="45"/>
-      <c r="K152" s="46"/>
+      <c r="B152" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C152" s="46"/>
+      <c r="D152" s="46"/>
+      <c r="E152" s="46"/>
+      <c r="F152" s="46"/>
+      <c r="G152" s="46"/>
+      <c r="H152" s="46"/>
+      <c r="I152" s="46"/>
+      <c r="J152" s="46"/>
+      <c r="K152" s="47"/>
     </row>
     <row r="153" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B153" s="13"/>
@@ -4113,32 +4185,32 @@
       <c r="K158" s="1"/>
     </row>
     <row r="159" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B159" s="51" t="s">
+      <c r="B159" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C159" s="52"/>
-      <c r="D159" s="52"/>
-      <c r="E159" s="52"/>
-      <c r="F159" s="52"/>
-      <c r="G159" s="52"/>
-      <c r="H159" s="52"/>
-      <c r="I159" s="52"/>
-      <c r="J159" s="52"/>
-      <c r="K159" s="53"/>
+      <c r="C159" s="49"/>
+      <c r="D159" s="49"/>
+      <c r="E159" s="49"/>
+      <c r="F159" s="49"/>
+      <c r="G159" s="49"/>
+      <c r="H159" s="49"/>
+      <c r="I159" s="49"/>
+      <c r="J159" s="49"/>
+      <c r="K159" s="50"/>
     </row>
     <row r="160" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B160" s="44" t="s">
+      <c r="B160" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C160" s="45"/>
-      <c r="D160" s="45"/>
-      <c r="E160" s="45"/>
-      <c r="F160" s="45"/>
-      <c r="G160" s="45"/>
-      <c r="H160" s="45"/>
-      <c r="I160" s="45"/>
-      <c r="J160" s="45"/>
-      <c r="K160" s="46"/>
+      <c r="C160" s="46"/>
+      <c r="D160" s="46"/>
+      <c r="E160" s="46"/>
+      <c r="F160" s="46"/>
+      <c r="G160" s="46"/>
+      <c r="H160" s="46"/>
+      <c r="I160" s="46"/>
+      <c r="J160" s="46"/>
+      <c r="K160" s="47"/>
     </row>
     <row r="161" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B161" s="3"/>
@@ -4155,7 +4227,7 @@
     <row r="162" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B162" s="3"/>
       <c r="C162" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D162" s="5"/>
       <c r="E162" s="5"/>
@@ -4179,18 +4251,18 @@
       <c r="K163" s="10"/>
     </row>
     <row r="164" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B164" s="44" t="s">
+      <c r="B164" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C164" s="45"/>
-      <c r="D164" s="45"/>
-      <c r="E164" s="45"/>
-      <c r="F164" s="45"/>
-      <c r="G164" s="45"/>
-      <c r="H164" s="45"/>
-      <c r="I164" s="45"/>
-      <c r="J164" s="45"/>
-      <c r="K164" s="46"/>
+      <c r="C164" s="46"/>
+      <c r="D164" s="46"/>
+      <c r="E164" s="46"/>
+      <c r="F164" s="46"/>
+      <c r="G164" s="46"/>
+      <c r="H164" s="46"/>
+      <c r="I164" s="46"/>
+      <c r="J164" s="46"/>
+      <c r="K164" s="47"/>
     </row>
     <row r="165" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B165" s="3"/>
@@ -4231,18 +4303,18 @@
       <c r="K167" s="10"/>
     </row>
     <row r="168" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B168" s="44" t="s">
+      <c r="B168" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C168" s="45"/>
-      <c r="D168" s="45"/>
-      <c r="E168" s="45"/>
-      <c r="F168" s="45"/>
-      <c r="G168" s="45"/>
-      <c r="H168" s="45"/>
-      <c r="I168" s="45"/>
-      <c r="J168" s="45"/>
-      <c r="K168" s="46"/>
+      <c r="C168" s="46"/>
+      <c r="D168" s="46"/>
+      <c r="E168" s="46"/>
+      <c r="F168" s="46"/>
+      <c r="G168" s="46"/>
+      <c r="H168" s="46"/>
+      <c r="I168" s="46"/>
+      <c r="J168" s="46"/>
+      <c r="K168" s="47"/>
     </row>
     <row r="169" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B169" s="15"/>
@@ -4283,18 +4355,18 @@
       <c r="K171" s="10"/>
     </row>
     <row r="172" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B172" s="44" t="s">
+      <c r="B172" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C172" s="45"/>
-      <c r="D172" s="45"/>
-      <c r="E172" s="45"/>
-      <c r="F172" s="45"/>
-      <c r="G172" s="45"/>
-      <c r="H172" s="45"/>
-      <c r="I172" s="45"/>
-      <c r="J172" s="45"/>
-      <c r="K172" s="46"/>
+      <c r="C172" s="46"/>
+      <c r="D172" s="46"/>
+      <c r="E172" s="46"/>
+      <c r="F172" s="46"/>
+      <c r="G172" s="46"/>
+      <c r="H172" s="46"/>
+      <c r="I172" s="46"/>
+      <c r="J172" s="46"/>
+      <c r="K172" s="47"/>
     </row>
     <row r="173" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B173" s="13"/>
@@ -4335,18 +4407,18 @@
       <c r="K175" s="10"/>
     </row>
     <row r="176" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B176" s="44" t="s">
+      <c r="B176" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="C176" s="45"/>
-      <c r="D176" s="45"/>
-      <c r="E176" s="45"/>
-      <c r="F176" s="45"/>
-      <c r="G176" s="45"/>
-      <c r="H176" s="45"/>
-      <c r="I176" s="45"/>
-      <c r="J176" s="45"/>
-      <c r="K176" s="46"/>
+      <c r="C176" s="46"/>
+      <c r="D176" s="46"/>
+      <c r="E176" s="46"/>
+      <c r="F176" s="46"/>
+      <c r="G176" s="46"/>
+      <c r="H176" s="46"/>
+      <c r="I176" s="46"/>
+      <c r="J176" s="46"/>
+      <c r="K176" s="47"/>
     </row>
     <row r="177" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B177" s="13"/>
@@ -4427,18 +4499,18 @@
       <c r="K181" s="10"/>
     </row>
     <row r="182" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B182" s="44" t="s">
+      <c r="B182" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C182" s="45"/>
-      <c r="D182" s="45"/>
-      <c r="E182" s="45"/>
-      <c r="F182" s="45"/>
-      <c r="G182" s="45"/>
-      <c r="H182" s="45"/>
-      <c r="I182" s="45"/>
-      <c r="J182" s="45"/>
-      <c r="K182" s="46"/>
+      <c r="C182" s="46"/>
+      <c r="D182" s="46"/>
+      <c r="E182" s="46"/>
+      <c r="F182" s="46"/>
+      <c r="G182" s="46"/>
+      <c r="H182" s="46"/>
+      <c r="I182" s="46"/>
+      <c r="J182" s="46"/>
+      <c r="K182" s="47"/>
     </row>
     <row r="183" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B183" s="13"/>
@@ -4525,18 +4597,18 @@
       <c r="K187" s="6"/>
     </row>
     <row r="188" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B188" s="44" t="s">
+      <c r="B188" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="C188" s="45"/>
-      <c r="D188" s="45"/>
-      <c r="E188" s="45"/>
-      <c r="F188" s="45"/>
-      <c r="G188" s="45"/>
-      <c r="H188" s="45"/>
-      <c r="I188" s="45"/>
-      <c r="J188" s="45"/>
-      <c r="K188" s="46"/>
+      <c r="C188" s="46"/>
+      <c r="D188" s="46"/>
+      <c r="E188" s="46"/>
+      <c r="F188" s="46"/>
+      <c r="G188" s="46"/>
+      <c r="H188" s="46"/>
+      <c r="I188" s="46"/>
+      <c r="J188" s="46"/>
+      <c r="K188" s="47"/>
     </row>
     <row r="189" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B189" s="13"/>
@@ -4635,32 +4707,32 @@
       <c r="K194" s="5"/>
     </row>
     <row r="195" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B195" s="51" t="s">
+      <c r="B195" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C195" s="52"/>
-      <c r="D195" s="52"/>
-      <c r="E195" s="52"/>
-      <c r="F195" s="52"/>
-      <c r="G195" s="52"/>
-      <c r="H195" s="52"/>
-      <c r="I195" s="52"/>
-      <c r="J195" s="52"/>
-      <c r="K195" s="53"/>
+      <c r="C195" s="49"/>
+      <c r="D195" s="49"/>
+      <c r="E195" s="49"/>
+      <c r="F195" s="49"/>
+      <c r="G195" s="49"/>
+      <c r="H195" s="49"/>
+      <c r="I195" s="49"/>
+      <c r="J195" s="49"/>
+      <c r="K195" s="50"/>
     </row>
     <row r="196" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B196" s="44" t="s">
+      <c r="B196" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C196" s="45"/>
-      <c r="D196" s="45"/>
-      <c r="E196" s="45"/>
-      <c r="F196" s="45"/>
-      <c r="G196" s="45"/>
-      <c r="H196" s="45"/>
-      <c r="I196" s="45"/>
-      <c r="J196" s="45"/>
-      <c r="K196" s="46"/>
+      <c r="C196" s="46"/>
+      <c r="D196" s="46"/>
+      <c r="E196" s="46"/>
+      <c r="F196" s="46"/>
+      <c r="G196" s="46"/>
+      <c r="H196" s="46"/>
+      <c r="I196" s="46"/>
+      <c r="J196" s="46"/>
+      <c r="K196" s="47"/>
     </row>
     <row r="197" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B197" s="3"/>
@@ -4677,7 +4749,7 @@
     <row r="198" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B198" s="3"/>
       <c r="C198" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D198" s="5"/>
       <c r="E198" s="5"/>
@@ -4701,18 +4773,18 @@
       <c r="K199" s="10"/>
     </row>
     <row r="200" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B200" s="44" t="s">
+      <c r="B200" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C200" s="45"/>
-      <c r="D200" s="45"/>
-      <c r="E200" s="45"/>
-      <c r="F200" s="45"/>
-      <c r="G200" s="45"/>
-      <c r="H200" s="45"/>
-      <c r="I200" s="45"/>
-      <c r="J200" s="45"/>
-      <c r="K200" s="46"/>
+      <c r="C200" s="46"/>
+      <c r="D200" s="46"/>
+      <c r="E200" s="46"/>
+      <c r="F200" s="46"/>
+      <c r="G200" s="46"/>
+      <c r="H200" s="46"/>
+      <c r="I200" s="46"/>
+      <c r="J200" s="46"/>
+      <c r="K200" s="47"/>
     </row>
     <row r="201" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B201" s="3"/>
@@ -4753,18 +4825,18 @@
       <c r="K203" s="10"/>
     </row>
     <row r="204" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B204" s="44" t="s">
+      <c r="B204" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C204" s="45"/>
-      <c r="D204" s="45"/>
-      <c r="E204" s="45"/>
-      <c r="F204" s="45"/>
-      <c r="G204" s="45"/>
-      <c r="H204" s="45"/>
-      <c r="I204" s="45"/>
-      <c r="J204" s="45"/>
-      <c r="K204" s="46"/>
+      <c r="C204" s="46"/>
+      <c r="D204" s="46"/>
+      <c r="E204" s="46"/>
+      <c r="F204" s="46"/>
+      <c r="G204" s="46"/>
+      <c r="H204" s="46"/>
+      <c r="I204" s="46"/>
+      <c r="J204" s="46"/>
+      <c r="K204" s="47"/>
     </row>
     <row r="205" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B205" s="15"/>
@@ -4805,18 +4877,18 @@
       <c r="K207" s="10"/>
     </row>
     <row r="208" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B208" s="44" t="s">
+      <c r="B208" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C208" s="45"/>
-      <c r="D208" s="45"/>
-      <c r="E208" s="45"/>
-      <c r="F208" s="45"/>
-      <c r="G208" s="45"/>
-      <c r="H208" s="45"/>
-      <c r="I208" s="45"/>
-      <c r="J208" s="45"/>
-      <c r="K208" s="46"/>
+      <c r="C208" s="46"/>
+      <c r="D208" s="46"/>
+      <c r="E208" s="46"/>
+      <c r="F208" s="46"/>
+      <c r="G208" s="46"/>
+      <c r="H208" s="46"/>
+      <c r="I208" s="46"/>
+      <c r="J208" s="46"/>
+      <c r="K208" s="47"/>
     </row>
     <row r="209" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B209" s="13"/>
@@ -4857,18 +4929,18 @@
       <c r="K211" s="10"/>
     </row>
     <row r="212" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B212" s="44" t="s">
+      <c r="B212" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="C212" s="45"/>
-      <c r="D212" s="45"/>
-      <c r="E212" s="45"/>
-      <c r="F212" s="45"/>
-      <c r="G212" s="45"/>
-      <c r="H212" s="45"/>
-      <c r="I212" s="45"/>
-      <c r="J212" s="45"/>
-      <c r="K212" s="46"/>
+      <c r="C212" s="46"/>
+      <c r="D212" s="46"/>
+      <c r="E212" s="46"/>
+      <c r="F212" s="46"/>
+      <c r="G212" s="46"/>
+      <c r="H212" s="46"/>
+      <c r="I212" s="46"/>
+      <c r="J212" s="46"/>
+      <c r="K212" s="47"/>
     </row>
     <row r="213" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B213" s="13"/>
@@ -4949,18 +5021,18 @@
       <c r="K217" s="10"/>
     </row>
     <row r="218" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B218" s="44" t="s">
+      <c r="B218" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C218" s="45"/>
-      <c r="D218" s="45"/>
-      <c r="E218" s="45"/>
-      <c r="F218" s="45"/>
-      <c r="G218" s="45"/>
-      <c r="H218" s="45"/>
-      <c r="I218" s="45"/>
-      <c r="J218" s="45"/>
-      <c r="K218" s="46"/>
+      <c r="C218" s="46"/>
+      <c r="D218" s="46"/>
+      <c r="E218" s="46"/>
+      <c r="F218" s="46"/>
+      <c r="G218" s="46"/>
+      <c r="H218" s="46"/>
+      <c r="I218" s="46"/>
+      <c r="J218" s="46"/>
+      <c r="K218" s="47"/>
     </row>
     <row r="219" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B219" s="13"/>
@@ -5047,18 +5119,18 @@
       <c r="K223" s="6"/>
     </row>
     <row r="224" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B224" s="44" t="s">
+      <c r="B224" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="C224" s="45"/>
-      <c r="D224" s="45"/>
-      <c r="E224" s="45"/>
-      <c r="F224" s="45"/>
-      <c r="G224" s="45"/>
-      <c r="H224" s="45"/>
-      <c r="I224" s="45"/>
-      <c r="J224" s="45"/>
-      <c r="K224" s="46"/>
+      <c r="C224" s="46"/>
+      <c r="D224" s="46"/>
+      <c r="E224" s="46"/>
+      <c r="F224" s="46"/>
+      <c r="G224" s="46"/>
+      <c r="H224" s="46"/>
+      <c r="I224" s="46"/>
+      <c r="J224" s="46"/>
+      <c r="K224" s="47"/>
     </row>
     <row r="225" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B225" s="13"/>
@@ -5326,31 +5398,24 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="B100:K100"/>
-    <mergeCell ref="B95:K95"/>
-    <mergeCell ref="B91:K91"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B212:K212"/>
-    <mergeCell ref="B116:K116"/>
+    <mergeCell ref="B55:K55"/>
+    <mergeCell ref="B50:K50"/>
+    <mergeCell ref="B123:K123"/>
+    <mergeCell ref="B124:K124"/>
     <mergeCell ref="B128:K128"/>
-    <mergeCell ref="B218:K218"/>
-    <mergeCell ref="B224:K224"/>
-    <mergeCell ref="B123:K123"/>
+    <mergeCell ref="B160:K160"/>
+    <mergeCell ref="B73:K73"/>
+    <mergeCell ref="B67:K67"/>
+    <mergeCell ref="B63:K63"/>
+    <mergeCell ref="B86:K86"/>
+    <mergeCell ref="B110:K110"/>
+    <mergeCell ref="B104:K104"/>
     <mergeCell ref="B132:K132"/>
     <mergeCell ref="B136:K136"/>
     <mergeCell ref="I138:J138"/>
     <mergeCell ref="B140:K140"/>
     <mergeCell ref="B146:K146"/>
     <mergeCell ref="B152:K152"/>
-    <mergeCell ref="B188:K188"/>
-    <mergeCell ref="B195:K195"/>
-    <mergeCell ref="B200:K200"/>
-    <mergeCell ref="B204:K204"/>
     <mergeCell ref="B208:K208"/>
     <mergeCell ref="B196:K196"/>
     <mergeCell ref="E33:H33"/>
@@ -5367,23 +5432,30 @@
     <mergeCell ref="B172:K172"/>
     <mergeCell ref="B176:K176"/>
     <mergeCell ref="B182:K182"/>
+    <mergeCell ref="B212:K212"/>
+    <mergeCell ref="B116:K116"/>
+    <mergeCell ref="B218:K218"/>
+    <mergeCell ref="B224:K224"/>
+    <mergeCell ref="B188:K188"/>
+    <mergeCell ref="B195:K195"/>
+    <mergeCell ref="B200:K200"/>
+    <mergeCell ref="B204:K204"/>
+    <mergeCell ref="B100:K100"/>
+    <mergeCell ref="B95:K95"/>
+    <mergeCell ref="B91:K91"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B4:K4"/>
     <mergeCell ref="B79:K79"/>
     <mergeCell ref="B5:K5"/>
     <mergeCell ref="B51:K51"/>
     <mergeCell ref="B87:K87"/>
-    <mergeCell ref="B124:K124"/>
-    <mergeCell ref="B160:K160"/>
-    <mergeCell ref="B73:K73"/>
-    <mergeCell ref="B67:K67"/>
-    <mergeCell ref="B63:K63"/>
     <mergeCell ref="B59:K59"/>
-    <mergeCell ref="B86:K86"/>
-    <mergeCell ref="B110:K110"/>
-    <mergeCell ref="B104:K104"/>
     <mergeCell ref="B43:K43"/>
     <mergeCell ref="B37:K37"/>
-    <mergeCell ref="B55:K55"/>
-    <mergeCell ref="B50:K50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5395,7 +5467,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5416,14 +5488,14 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="A2" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -5435,12 +5507,12 @@
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="51" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="B4" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="50"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5455,10 +5527,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>67</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>68</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="1"/>
@@ -5491,10 +5563,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
       <c r="C9" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="1"/>
@@ -5541,12 +5613,12 @@
     </row>
     <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="53"/>
+      <c r="B14" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="50"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -5561,10 +5633,10 @@
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="1"/>
@@ -5609,7 +5681,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="25" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Forgot to update com protocol
Very important stuff
</commit_message>
<xml_diff>
--- a/Laser_Engraver_Embedded/communication_protocol.xlsx
+++ b/Laser_Engraver_Embedded/communication_protocol.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="450" yWindow="255" windowWidth="20895" windowHeight="14505"/>
+    <workbookView xWindow="450" yWindow="255" windowWidth="20895" windowHeight="14505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Communication Flow" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="98">
   <si>
     <t>Bit7</t>
   </si>
@@ -119,9 +119,6 @@
     <t>0x0D</t>
   </si>
   <si>
-    <t>MSP_INIT</t>
-  </si>
-  <si>
     <t>0x01</t>
   </si>
   <si>
@@ -248,9 +245,6 @@
     <t>MSP -&gt; PI</t>
   </si>
   <si>
-    <t>MSP has correctly initialized and is ready to start burning an image</t>
-  </si>
-  <si>
     <t xml:space="preserve">BURN </t>
   </si>
   <si>
@@ -293,9 +287,6 @@
     <t>Start a Picture</t>
   </si>
   <si>
-    <t>MSP is Initialized</t>
-  </si>
-  <si>
     <t>Burn a Pixel</t>
   </si>
   <si>
@@ -321,6 +312,9 @@
   </si>
   <si>
     <t>Pi has correctly initialized and is ready to start communicating with the MSP</t>
+  </si>
+  <si>
+    <t>Pi is Initialized</t>
   </si>
 </sst>
 </file>
@@ -719,16 +713,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1073,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,25 +1104,25 @@
       <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
+      <c r="A2" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
-      <c r="J2" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+      <c r="J2" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
@@ -1151,13 +1145,13 @@
       <c r="A4" s="24"/>
       <c r="B4" s="22"/>
       <c r="C4" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>73</v>
-      </c>
       <c r="E4" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="24"/>
@@ -1166,10 +1160,10 @@
       <c r="J4" s="24"/>
       <c r="K4" s="22"/>
       <c r="L4" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M4" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N4" s="23"/>
       <c r="O4" s="24"/>
@@ -1195,7 +1189,7 @@
       <c r="A6" s="24"/>
       <c r="B6" s="29"/>
       <c r="C6" s="42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D6" s="42"/>
       <c r="E6" s="42"/>
@@ -1206,7 +1200,7 @@
       <c r="J6" s="24"/>
       <c r="K6" s="29"/>
       <c r="L6" s="42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M6" s="42"/>
       <c r="N6" s="30"/>
@@ -1233,13 +1227,13 @@
       <c r="A8" s="24"/>
       <c r="B8" s="26"/>
       <c r="C8" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="24"/>
@@ -1248,90 +1242,90 @@
       <c r="J8" s="24"/>
       <c r="K8" s="26"/>
       <c r="L8" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="N8" s="28"/>
       <c r="O8" s="24"/>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>32</v>
-      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="6"/>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="M9" s="25" t="s">
-        <v>90</v>
-      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="25"/>
       <c r="N9" s="6"/>
       <c r="O9" s="24"/>
     </row>
-    <row r="10" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="C10" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="6"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="25"/>
+      <c r="L10" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M10" s="44"/>
       <c r="N10" s="6"/>
       <c r="O10" s="24"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+      <c r="C11" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>33</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="M11" s="43"/>
+      <c r="L11" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="M11" s="37" t="s">
+        <v>87</v>
+      </c>
       <c r="N11" s="6"/>
       <c r="O11" s="24"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>34</v>
+      <c r="C12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>25</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="24"/>
@@ -1339,11 +1333,11 @@
       <c r="I12" s="24"/>
       <c r="J12" s="24"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="M12" s="37" t="s">
-        <v>89</v>
+      <c r="L12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>88</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="24"/>
@@ -1352,13 +1346,13 @@
       <c r="A13" s="24"/>
       <c r="B13" s="3"/>
       <c r="C13" s="13" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>78</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="24"/>
@@ -1367,10 +1361,10 @@
       <c r="J13" s="24"/>
       <c r="K13" s="3"/>
       <c r="L13" s="13" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="M13" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="24"/>
@@ -1379,13 +1373,13 @@
       <c r="A14" s="24"/>
       <c r="B14" s="3"/>
       <c r="C14" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="38" t="s">
         <v>74</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>28</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="24"/>
@@ -1394,10 +1388,10 @@
       <c r="J14" s="24"/>
       <c r="K14" s="3"/>
       <c r="L14" s="13" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M14" s="38" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="24"/>
@@ -1406,13 +1400,13 @@
       <c r="A15" s="24"/>
       <c r="B15" s="3"/>
       <c r="C15" s="13" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="24"/>
@@ -1421,10 +1415,10 @@
       <c r="J15" s="24"/>
       <c r="K15" s="3"/>
       <c r="L15" s="13" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="M15" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="24"/>
@@ -1433,13 +1427,13 @@
       <c r="A16" s="24"/>
       <c r="B16" s="3"/>
       <c r="C16" s="13" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="E16" s="38" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="24"/>
@@ -1448,10 +1442,10 @@
       <c r="J16" s="24"/>
       <c r="K16" s="3"/>
       <c r="L16" s="13" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="M16" s="38" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="24"/>
@@ -1460,13 +1454,13 @@
       <c r="A17" s="24"/>
       <c r="B17" s="3"/>
       <c r="C17" s="13" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="24"/>
@@ -1475,10 +1469,10 @@
       <c r="J17" s="24"/>
       <c r="K17" s="3"/>
       <c r="L17" s="13" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="M17" s="38" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="24"/>
@@ -1486,14 +1480,14 @@
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="38" t="s">
-        <v>77</v>
+      <c r="E18" s="39" t="s">
+        <v>35</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="24"/>
@@ -1501,261 +1495,234 @@
       <c r="I18" s="24"/>
       <c r="J18" s="24"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="M18" s="38" t="s">
-        <v>93</v>
+      <c r="L18" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="M18" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="24"/>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>36</v>
-      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="6"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="M19" s="39" t="s">
-        <v>94</v>
-      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="25"/>
       <c r="N19" s="6"/>
       <c r="O19" s="24"/>
     </row>
-    <row r="20" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
+      <c r="C20" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="6"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="25"/>
+      <c r="L20" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M20" s="44"/>
       <c r="N20" s="6"/>
       <c r="O20" s="24"/>
     </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
       <c r="F21" s="6"/>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
       <c r="J21" s="24"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="M21" s="43"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="25"/>
       <c r="N21" s="6"/>
       <c r="O21" s="24"/>
     </row>
-    <row r="22" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
+      <c r="C22" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
       <c r="F22" s="6"/>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
       <c r="J22" s="24"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="25"/>
+      <c r="L22" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M22" s="44"/>
       <c r="N22" s="6"/>
       <c r="O22" s="24"/>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
       <c r="F23" s="6"/>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
       <c r="I23" s="24"/>
       <c r="J23" s="24"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="M23" s="43"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="25"/>
       <c r="N23" s="6"/>
       <c r="O23" s="24"/>
     </row>
-    <row r="24" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
+      <c r="C24" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="6"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
       <c r="I24" s="24"/>
       <c r="J24" s="24"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="25"/>
+      <c r="L24" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" s="41"/>
       <c r="N24" s="6"/>
       <c r="O24" s="24"/>
     </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
       <c r="F25" s="6"/>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
       <c r="J25" s="24"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="M25" s="44"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="25"/>
       <c r="N25" s="6"/>
       <c r="O25" s="24"/>
     </row>
-    <row r="26" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="6"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="30"/>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
       <c r="I26" s="24"/>
       <c r="J26" s="24"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="6"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="M26" s="42"/>
+      <c r="N26" s="30"/>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="30"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="10"/>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
       <c r="I27" s="24"/>
       <c r="J27" s="24"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="M27" s="42"/>
-      <c r="N27" s="30"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="10"/>
       <c r="O27" s="24"/>
     </row>
-    <row r="28" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="10"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
       <c r="I28" s="24"/>
       <c r="J28" s="24"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="10"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
       <c r="O28" s="24"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="24"/>
       <c r="H29" s="24"/>
       <c r="I29" s="24"/>
       <c r="J29" s="24"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
       <c r="O29" s="24"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C24:E24"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L22:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1766,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L244"/>
   <sheetViews>
-    <sheetView topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R135" sqref="R135"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1795,17 +1762,17 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -1836,7 +1803,7 @@
     </row>
     <row r="5" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
@@ -1863,7 +1830,7 @@
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1978,11 +1945,11 @@
         <v>8</v>
       </c>
       <c r="F15" s="53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G15" s="55"/>
       <c r="H15" s="53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I15" s="54"/>
       <c r="J15" s="55"/>
@@ -2033,7 +2000,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="54"/>
       <c r="E18" s="54"/>
@@ -2089,11 +2056,11 @@
         <v>10</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="55"/>
       <c r="E21" s="53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" s="54"/>
       <c r="G21" s="54"/>
@@ -2147,7 +2114,7 @@
         <v>9</v>
       </c>
       <c r="C24" s="53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="54"/>
       <c r="E24" s="54"/>
@@ -2156,7 +2123,7 @@
       <c r="H24" s="54"/>
       <c r="I24" s="55"/>
       <c r="J24" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K24" s="6"/>
     </row>
@@ -2254,7 +2221,7 @@
     </row>
     <row r="31" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="46"/>
@@ -2293,7 +2260,7 @@
       <c r="G33" s="52"/>
       <c r="H33" s="52"/>
       <c r="I33" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J33" s="14" t="s">
         <v>20</v>
@@ -2321,7 +2288,7 @@
         <v>9</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J34" s="12" t="s">
         <v>16</v>
@@ -2370,7 +2337,7 @@
     </row>
     <row r="37" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" s="46"/>
       <c r="D37" s="46"/>
@@ -2420,7 +2387,7 @@
         <v>15</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>26</v>
@@ -2468,7 +2435,7 @@
     </row>
     <row r="43" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="46"/>
       <c r="D43" s="46"/>
@@ -2518,7 +2485,7 @@
         <v>15</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>26</v>
@@ -2592,7 +2559,7 @@
     </row>
     <row r="51" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" s="46"/>
       <c r="D51" s="46"/>
@@ -2619,7 +2586,7 @@
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
       <c r="C53" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -2800,7 +2767,7 @@
     </row>
     <row r="67" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C67" s="46"/>
       <c r="D67" s="46"/>
@@ -2892,7 +2859,7 @@
     </row>
     <row r="73" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C73" s="46"/>
       <c r="D73" s="46"/>
@@ -2942,7 +2909,7 @@
         <v>15</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E76" s="12" t="s">
         <v>29</v>
@@ -2990,7 +2957,7 @@
     </row>
     <row r="79" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B79" s="45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C79" s="46"/>
       <c r="D79" s="46"/>
@@ -3040,7 +3007,7 @@
         <v>15</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E82" s="12" t="s">
         <v>29</v>
@@ -3114,7 +3081,7 @@
     </row>
     <row r="87" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B87" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C87" s="46"/>
       <c r="D87" s="46"/>
@@ -3141,7 +3108,7 @@
     <row r="89" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B89" s="3"/>
       <c r="C89" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -3247,7 +3214,7 @@
         <v>9</v>
       </c>
       <c r="C97" s="53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D97" s="54"/>
       <c r="E97" s="54"/>
@@ -3352,7 +3319,7 @@
     </row>
     <row r="104" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B104" s="45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C104" s="46"/>
       <c r="D104" s="46"/>
@@ -3388,7 +3355,7 @@
         <v>19</v>
       </c>
       <c r="F106" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G106" s="14" t="s">
         <v>20</v>
@@ -3410,7 +3377,7 @@
         <v>9</v>
       </c>
       <c r="F107" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G107" s="12" t="s">
         <v>16</v>
@@ -3456,7 +3423,7 @@
     </row>
     <row r="110" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B110" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C110" s="46"/>
       <c r="D110" s="46"/>
@@ -3506,7 +3473,7 @@
         <v>15</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E113" s="12" t="s">
         <v>31</v>
@@ -3554,7 +3521,7 @@
     </row>
     <row r="116" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B116" s="45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C116" s="46"/>
       <c r="D116" s="46"/>
@@ -3604,7 +3571,7 @@
         <v>15</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E119" s="12" t="s">
         <v>31</v>
@@ -3664,7 +3631,7 @@
     </row>
     <row r="123" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B123" s="48" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C123" s="49"/>
       <c r="D123" s="49"/>
@@ -3678,7 +3645,7 @@
     </row>
     <row r="124" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B124" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C124" s="46"/>
       <c r="D124" s="46"/>
@@ -3705,7 +3672,7 @@
     <row r="126" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B126" s="3"/>
       <c r="C126" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
@@ -3757,7 +3724,7 @@
     <row r="130" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B130" s="3"/>
       <c r="C130" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D130" s="5"/>
       <c r="E130" s="5"/>
@@ -3886,7 +3853,7 @@
     </row>
     <row r="140" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B140" s="45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C140" s="46"/>
       <c r="D140" s="46"/>
@@ -3934,7 +3901,7 @@
         <v>15</v>
       </c>
       <c r="D143" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E143" s="12" t="s">
         <v>16</v>
@@ -3978,7 +3945,7 @@
     </row>
     <row r="146" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B146" s="45" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C146" s="46"/>
       <c r="D146" s="46"/>
@@ -4028,10 +3995,10 @@
         <v>15</v>
       </c>
       <c r="D149" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E149" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F149" s="12" t="s">
         <v>16</v>
@@ -4076,7 +4043,7 @@
     </row>
     <row r="152" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B152" s="45" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C152" s="46"/>
       <c r="D152" s="46"/>
@@ -4126,10 +4093,10 @@
         <v>15</v>
       </c>
       <c r="D155" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E155" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F155" s="12" t="s">
         <v>16</v>
@@ -4186,7 +4153,7 @@
     </row>
     <row r="159" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B159" s="48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C159" s="49"/>
       <c r="D159" s="49"/>
@@ -4200,7 +4167,7 @@
     </row>
     <row r="160" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B160" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C160" s="46"/>
       <c r="D160" s="46"/>
@@ -4227,7 +4194,7 @@
     <row r="162" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B162" s="3"/>
       <c r="C162" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D162" s="5"/>
       <c r="E162" s="5"/>
@@ -4279,7 +4246,7 @@
     <row r="166" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B166" s="3"/>
       <c r="C166" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D166" s="5"/>
       <c r="E166" s="5"/>
@@ -4408,7 +4375,7 @@
     </row>
     <row r="176" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B176" s="45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C176" s="46"/>
       <c r="D176" s="46"/>
@@ -4456,7 +4423,7 @@
         <v>15</v>
       </c>
       <c r="D179" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E179" s="12" t="s">
         <v>16</v>
@@ -4500,7 +4467,7 @@
     </row>
     <row r="182" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B182" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C182" s="46"/>
       <c r="D182" s="46"/>
@@ -4550,10 +4517,10 @@
         <v>15</v>
       </c>
       <c r="D185" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E185" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F185" s="12" t="s">
         <v>16</v>
@@ -4598,7 +4565,7 @@
     </row>
     <row r="188" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B188" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C188" s="46"/>
       <c r="D188" s="46"/>
@@ -4648,10 +4615,10 @@
         <v>15</v>
       </c>
       <c r="D191" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E191" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F191" s="12" t="s">
         <v>16</v>
@@ -4708,7 +4675,7 @@
     </row>
     <row r="195" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B195" s="48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C195" s="49"/>
       <c r="D195" s="49"/>
@@ -4722,7 +4689,7 @@
     </row>
     <row r="196" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B196" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C196" s="46"/>
       <c r="D196" s="46"/>
@@ -4749,7 +4716,7 @@
     <row r="198" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B198" s="3"/>
       <c r="C198" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D198" s="5"/>
       <c r="E198" s="5"/>
@@ -4801,7 +4768,7 @@
     <row r="202" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B202" s="3"/>
       <c r="C202" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D202" s="5"/>
       <c r="E202" s="5"/>
@@ -4930,7 +4897,7 @@
     </row>
     <row r="212" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B212" s="45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C212" s="46"/>
       <c r="D212" s="46"/>
@@ -4978,7 +4945,7 @@
         <v>15</v>
       </c>
       <c r="D215" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E215" s="12" t="s">
         <v>16</v>
@@ -5022,7 +4989,7 @@
     </row>
     <row r="218" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B218" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C218" s="46"/>
       <c r="D218" s="46"/>
@@ -5072,10 +5039,10 @@
         <v>15</v>
       </c>
       <c r="D221" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E221" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F221" s="12" t="s">
         <v>16</v>
@@ -5120,7 +5087,7 @@
     </row>
     <row r="224" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B224" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C224" s="46"/>
       <c r="D224" s="46"/>
@@ -5170,10 +5137,10 @@
         <v>15</v>
       </c>
       <c r="D227" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E227" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F227" s="12" t="s">
         <v>16</v>
@@ -5398,24 +5365,23 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="B55:K55"/>
-    <mergeCell ref="B50:K50"/>
-    <mergeCell ref="B123:K123"/>
-    <mergeCell ref="B124:K124"/>
-    <mergeCell ref="B128:K128"/>
-    <mergeCell ref="B160:K160"/>
-    <mergeCell ref="B73:K73"/>
-    <mergeCell ref="B67:K67"/>
-    <mergeCell ref="B63:K63"/>
-    <mergeCell ref="B86:K86"/>
-    <mergeCell ref="B110:K110"/>
-    <mergeCell ref="B104:K104"/>
-    <mergeCell ref="B132:K132"/>
-    <mergeCell ref="B136:K136"/>
-    <mergeCell ref="I138:J138"/>
-    <mergeCell ref="B140:K140"/>
-    <mergeCell ref="B146:K146"/>
-    <mergeCell ref="B152:K152"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B37:K37"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B212:K212"/>
+    <mergeCell ref="B116:K116"/>
+    <mergeCell ref="B218:K218"/>
+    <mergeCell ref="B224:K224"/>
+    <mergeCell ref="B188:K188"/>
+    <mergeCell ref="B195:K195"/>
+    <mergeCell ref="B200:K200"/>
+    <mergeCell ref="B204:K204"/>
     <mergeCell ref="B208:K208"/>
     <mergeCell ref="B196:K196"/>
     <mergeCell ref="E33:H33"/>
@@ -5432,30 +5398,31 @@
     <mergeCell ref="B172:K172"/>
     <mergeCell ref="B176:K176"/>
     <mergeCell ref="B182:K182"/>
-    <mergeCell ref="B212:K212"/>
-    <mergeCell ref="B116:K116"/>
-    <mergeCell ref="B218:K218"/>
-    <mergeCell ref="B224:K224"/>
-    <mergeCell ref="B188:K188"/>
-    <mergeCell ref="B195:K195"/>
-    <mergeCell ref="B200:K200"/>
-    <mergeCell ref="B204:K204"/>
+    <mergeCell ref="B160:K160"/>
+    <mergeCell ref="B73:K73"/>
+    <mergeCell ref="B67:K67"/>
+    <mergeCell ref="B63:K63"/>
+    <mergeCell ref="B86:K86"/>
+    <mergeCell ref="B110:K110"/>
+    <mergeCell ref="B104:K104"/>
+    <mergeCell ref="B132:K132"/>
+    <mergeCell ref="B136:K136"/>
+    <mergeCell ref="I138:J138"/>
+    <mergeCell ref="B140:K140"/>
+    <mergeCell ref="B146:K146"/>
+    <mergeCell ref="B152:K152"/>
     <mergeCell ref="B100:K100"/>
     <mergeCell ref="B95:K95"/>
     <mergeCell ref="B91:K91"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B55:K55"/>
+    <mergeCell ref="B50:K50"/>
+    <mergeCell ref="B123:K123"/>
+    <mergeCell ref="B124:K124"/>
+    <mergeCell ref="B128:K128"/>
     <mergeCell ref="B79:K79"/>
-    <mergeCell ref="B5:K5"/>
     <mergeCell ref="B51:K51"/>
     <mergeCell ref="B87:K87"/>
     <mergeCell ref="B59:K59"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B37:K37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5466,8 +5433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5488,14 +5455,14 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="A2" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -5508,7 +5475,7 @@
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="49"/>
@@ -5527,10 +5494,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>66</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>67</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="1"/>
@@ -5563,10 +5530,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
       <c r="C9" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="1"/>
@@ -5578,7 +5545,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="1"/>
@@ -5590,7 +5557,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="1"/>
@@ -5614,7 +5581,7 @@
     <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
@@ -5633,10 +5600,10 @@
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="1"/>
@@ -5681,10 +5648,10 @@
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="25" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="1"/>
@@ -5693,10 +5660,10 @@
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="1"/>
@@ -5705,10 +5672,10 @@
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="1"/>

</xml_diff>